<commit_message>
executável ok, progresso na planilha
</commit_message>
<xml_diff>
--- a/SA38 Test.xlsx
+++ b/SA38 Test.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosga\Documents\Python\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6CC634-2EA2-4128-BA6D-70E4086CDF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheetName" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -253,11 +259,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,13 +327,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -365,7 +379,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -399,6 +413,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -433,9 +448,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -608,50 +624,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" customWidth="1"/>
-    <col min="12" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" customWidth="1"/>
-    <col min="21" max="24" width="14.7109375" customWidth="1"/>
-    <col min="25" max="25" width="15.7109375" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" customWidth="1"/>
-    <col min="27" max="27" width="14.7109375" customWidth="1"/>
-    <col min="28" max="28" width="15.7109375" customWidth="1"/>
-    <col min="29" max="29" width="40.7109375" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" customWidth="1"/>
-    <col min="32" max="32" width="13.7109375" customWidth="1"/>
-    <col min="33" max="33" width="15.7109375" customWidth="1"/>
-    <col min="34" max="34" width="11.7109375" customWidth="1"/>
-    <col min="35" max="35" width="6.7109375" customWidth="1"/>
-    <col min="36" max="37" width="13.7109375" customWidth="1"/>
-    <col min="38" max="38" width="14.7109375" customWidth="1"/>
-    <col min="39" max="39" width="7.7109375" customWidth="1"/>
-    <col min="40" max="40" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="4.6640625" customWidth="1"/>
+    <col min="12" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" customWidth="1"/>
+    <col min="21" max="24" width="14.6640625" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" customWidth="1"/>
+    <col min="27" max="27" width="14.6640625" customWidth="1"/>
+    <col min="28" max="28" width="15.6640625" customWidth="1"/>
+    <col min="29" max="29" width="40.6640625" customWidth="1"/>
+    <col min="30" max="30" width="13.6640625" customWidth="1"/>
+    <col min="31" max="31" width="14.6640625" customWidth="1"/>
+    <col min="32" max="32" width="13.6640625" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" customWidth="1"/>
+    <col min="34" max="34" width="11.6640625" customWidth="1"/>
+    <col min="35" max="35" width="6.6640625" customWidth="1"/>
+    <col min="36" max="37" width="13.6640625" customWidth="1"/>
+    <col min="38" max="38" width="14.6640625" customWidth="1"/>
+    <col min="39" max="39" width="7.6640625" customWidth="1"/>
+    <col min="40" max="40" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,7 +791,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -895,7 +913,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1017,7 +1035,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1139,7 +1157,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1261,7 +1279,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1383,7 +1401,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1505,7 +1523,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1627,7 +1645,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1749,7 +1767,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1790,7 +1808,7 @@
         <v>68</v>
       </c>
       <c r="N10">
-        <v>36.27</v>
+        <v>36.270000000000003</v>
       </c>
       <c r="O10" t="s">
         <v>69</v>
@@ -1871,7 +1889,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1912,7 +1930,7 @@
         <v>68</v>
       </c>
       <c r="N11">
-        <v>36.27</v>
+        <v>36.270000000000003</v>
       </c>
       <c r="O11" t="s">
         <v>69</v>
@@ -1993,7 +2011,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2034,7 +2052,7 @@
         <v>68</v>
       </c>
       <c r="N12">
-        <v>36.27</v>
+        <v>36.270000000000003</v>
       </c>
       <c r="O12" t="s">
         <v>69</v>
@@ -2115,7 +2133,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2156,7 +2174,7 @@
         <v>68</v>
       </c>
       <c r="N13">
-        <v>36.27</v>
+        <v>36.270000000000003</v>
       </c>
       <c r="O13" t="s">
         <v>69</v>
@@ -2237,7 +2255,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2278,7 +2296,7 @@
         <v>68</v>
       </c>
       <c r="N14">
-        <v>36.27</v>
+        <v>36.270000000000003</v>
       </c>
       <c r="O14" t="s">
         <v>69</v>
@@ -2359,7 +2377,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -2481,7 +2499,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2603,7 +2621,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2656,7 +2674,7 @@
         <v>74</v>
       </c>
       <c r="R17">
-        <v>4736.64</v>
+        <v>4736.6400000000003</v>
       </c>
       <c r="S17" t="s">
         <v>48</v>
@@ -2725,7 +2743,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -2847,7 +2865,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -2969,7 +2987,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -3091,7 +3109,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3213,7 +3231,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -3335,7 +3353,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -3457,7 +3475,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -3579,7 +3597,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3701,7 +3719,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -3823,7 +3841,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -3945,7 +3963,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -4067,7 +4085,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -4108,7 +4126,7 @@
         <v>68</v>
       </c>
       <c r="N29">
-        <v>37.77</v>
+        <v>37.770000000000003</v>
       </c>
       <c r="O29" t="s">
         <v>69</v>
@@ -4189,7 +4207,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -4230,7 +4248,7 @@
         <v>68</v>
       </c>
       <c r="N30">
-        <v>37.77</v>
+        <v>37.770000000000003</v>
       </c>
       <c r="O30" t="s">
         <v>69</v>
@@ -4311,7 +4329,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -4352,7 +4370,7 @@
         <v>68</v>
       </c>
       <c r="N31">
-        <v>37.77</v>
+        <v>37.770000000000003</v>
       </c>
       <c r="O31" t="s">
         <v>69</v>
@@ -4433,7 +4451,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -4474,7 +4492,7 @@
         <v>68</v>
       </c>
       <c r="N32">
-        <v>37.77</v>
+        <v>37.770000000000003</v>
       </c>
       <c r="O32" t="s">
         <v>69</v>
@@ -4555,7 +4573,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4596,7 +4614,7 @@
         <v>68</v>
       </c>
       <c r="N33">
-        <v>37.77</v>
+        <v>37.770000000000003</v>
       </c>
       <c r="O33" t="s">
         <v>69</v>
@@ -4677,7 +4695,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -4718,7 +4736,7 @@
         <v>68</v>
       </c>
       <c r="N34">
-        <v>37.77</v>
+        <v>37.770000000000003</v>
       </c>
       <c r="O34" t="s">
         <v>69</v>

</xml_diff>